<commit_message>
Data for dose response curves added
</commit_message>
<xml_diff>
--- a/data/Nuttal2008/Nuttal2008.xlsx
+++ b/data/Nuttal2008/Nuttal2008.xlsx
@@ -496,13 +496,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>87840</xdr:colOff>
+      <xdr:colOff>304920</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>406440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>583920</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>21960</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
@@ -533,13 +533,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>127440</xdr:colOff>
+      <xdr:colOff>344520</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>136440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>82080</xdr:colOff>
+      <xdr:colOff>299160</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
@@ -570,13 +570,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>110160</xdr:colOff>
+      <xdr:colOff>327240</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>116280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>592200</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>30240</xdr:colOff>
       <xdr:row>87</xdr:row>
       <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
@@ -615,7 +615,11 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R20" activeCellId="0" sqref="R20"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -632,7 +636,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="12.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="11.04"/>
   </cols>
   <sheetData>

</xml_diff>